<commit_message>
improved code readability and now the code runs through every pdf in the samples folder
</commit_message>
<xml_diff>
--- a/resumo.xlsx
+++ b/resumo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\valorizacaotoexcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\resumo_valorizacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94101E5C-C6BD-42A2-BD6E-FEA6E66EBD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5201F5DD-BF6A-406D-8AC6-7339320FE2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DATA</t>
   </si>
@@ -50,18 +50,6 @@
   </si>
   <si>
     <t>VALOR TOTAL</t>
-  </si>
-  <si>
-    <t>05/12/2023</t>
-  </si>
-  <si>
-    <t>ANDERSON CAMBE</t>
-  </si>
-  <si>
-    <t>Vivian Pereira Costa</t>
-  </si>
-  <si>
-    <t>118.539.189-46</t>
   </si>
 </sst>
 </file>
@@ -426,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K411"/>
+  <dimension ref="B2:K509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,100 +464,40 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5">
-        <v>3.4849999999999999</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1.119</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="J3" s="3">
-        <v>158.01</v>
-      </c>
-      <c r="K3" s="3">
-        <v>550.66</v>
-      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="5">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G4" s="6">
-        <v>2.5070000000000001</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="J4" s="3">
-        <v>412.56</v>
-      </c>
-      <c r="K4" s="3">
-        <v>474.44</v>
-      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1.67</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1.2769999999999999</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="J5" s="3">
-        <v>203.5</v>
-      </c>
-      <c r="K5" s="3">
-        <v>339.85</v>
-      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
@@ -5443,6 +5371,1182 @@
       <c r="J411" s="3"/>
       <c r="K411" s="3"/>
     </row>
+    <row r="412" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B412" s="4"/>
+      <c r="C412" s="2"/>
+      <c r="D412" s="2"/>
+      <c r="E412" s="2"/>
+      <c r="F412" s="5"/>
+      <c r="G412" s="6"/>
+      <c r="H412" s="6"/>
+      <c r="I412" s="6"/>
+      <c r="J412" s="3"/>
+      <c r="K412" s="3"/>
+    </row>
+    <row r="413" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B413" s="4"/>
+      <c r="C413" s="2"/>
+      <c r="D413" s="2"/>
+      <c r="E413" s="2"/>
+      <c r="F413" s="5"/>
+      <c r="G413" s="6"/>
+      <c r="H413" s="6"/>
+      <c r="I413" s="6"/>
+      <c r="J413" s="3"/>
+      <c r="K413" s="3"/>
+    </row>
+    <row r="414" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B414" s="4"/>
+      <c r="C414" s="2"/>
+      <c r="D414" s="2"/>
+      <c r="E414" s="2"/>
+      <c r="F414" s="5"/>
+      <c r="G414" s="6"/>
+      <c r="H414" s="6"/>
+      <c r="I414" s="6"/>
+      <c r="J414" s="3"/>
+      <c r="K414" s="3"/>
+    </row>
+    <row r="415" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B415" s="4"/>
+      <c r="C415" s="2"/>
+      <c r="D415" s="2"/>
+      <c r="E415" s="2"/>
+      <c r="F415" s="5"/>
+      <c r="G415" s="6"/>
+      <c r="H415" s="6"/>
+      <c r="I415" s="6"/>
+      <c r="J415" s="3"/>
+      <c r="K415" s="3"/>
+    </row>
+    <row r="416" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B416" s="4"/>
+      <c r="C416" s="2"/>
+      <c r="D416" s="2"/>
+      <c r="E416" s="2"/>
+      <c r="F416" s="5"/>
+      <c r="G416" s="6"/>
+      <c r="H416" s="6"/>
+      <c r="I416" s="6"/>
+      <c r="J416" s="3"/>
+      <c r="K416" s="3"/>
+    </row>
+    <row r="417" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B417" s="4"/>
+      <c r="C417" s="2"/>
+      <c r="D417" s="2"/>
+      <c r="E417" s="2"/>
+      <c r="F417" s="5"/>
+      <c r="G417" s="6"/>
+      <c r="H417" s="6"/>
+      <c r="I417" s="6"/>
+      <c r="J417" s="3"/>
+      <c r="K417" s="3"/>
+    </row>
+    <row r="418" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B418" s="4"/>
+      <c r="C418" s="2"/>
+      <c r="D418" s="2"/>
+      <c r="E418" s="2"/>
+      <c r="F418" s="5"/>
+      <c r="G418" s="6"/>
+      <c r="H418" s="6"/>
+      <c r="I418" s="6"/>
+      <c r="J418" s="3"/>
+      <c r="K418" s="3"/>
+    </row>
+    <row r="419" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B419" s="4"/>
+      <c r="C419" s="2"/>
+      <c r="D419" s="2"/>
+      <c r="E419" s="2"/>
+      <c r="F419" s="5"/>
+      <c r="G419" s="6"/>
+      <c r="H419" s="6"/>
+      <c r="I419" s="6"/>
+      <c r="J419" s="3"/>
+      <c r="K419" s="3"/>
+    </row>
+    <row r="420" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B420" s="4"/>
+      <c r="C420" s="2"/>
+      <c r="D420" s="2"/>
+      <c r="E420" s="2"/>
+      <c r="F420" s="5"/>
+      <c r="G420" s="6"/>
+      <c r="H420" s="6"/>
+      <c r="I420" s="6"/>
+      <c r="J420" s="3"/>
+      <c r="K420" s="3"/>
+    </row>
+    <row r="421" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B421" s="4"/>
+      <c r="C421" s="2"/>
+      <c r="D421" s="2"/>
+      <c r="E421" s="2"/>
+      <c r="F421" s="5"/>
+      <c r="G421" s="6"/>
+      <c r="H421" s="6"/>
+      <c r="I421" s="6"/>
+      <c r="J421" s="3"/>
+      <c r="K421" s="3"/>
+    </row>
+    <row r="422" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B422" s="4"/>
+      <c r="C422" s="2"/>
+      <c r="D422" s="2"/>
+      <c r="E422" s="2"/>
+      <c r="F422" s="5"/>
+      <c r="G422" s="6"/>
+      <c r="H422" s="6"/>
+      <c r="I422" s="6"/>
+      <c r="J422" s="3"/>
+      <c r="K422" s="3"/>
+    </row>
+    <row r="423" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B423" s="4"/>
+      <c r="C423" s="2"/>
+      <c r="D423" s="2"/>
+      <c r="E423" s="2"/>
+      <c r="F423" s="5"/>
+      <c r="G423" s="6"/>
+      <c r="H423" s="6"/>
+      <c r="I423" s="6"/>
+      <c r="J423" s="3"/>
+      <c r="K423" s="3"/>
+    </row>
+    <row r="424" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B424" s="4"/>
+      <c r="C424" s="2"/>
+      <c r="D424" s="2"/>
+      <c r="E424" s="2"/>
+      <c r="F424" s="5"/>
+      <c r="G424" s="6"/>
+      <c r="H424" s="6"/>
+      <c r="I424" s="6"/>
+      <c r="J424" s="3"/>
+      <c r="K424" s="3"/>
+    </row>
+    <row r="425" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B425" s="4"/>
+      <c r="C425" s="2"/>
+      <c r="D425" s="2"/>
+      <c r="E425" s="2"/>
+      <c r="F425" s="5"/>
+      <c r="G425" s="6"/>
+      <c r="H425" s="6"/>
+      <c r="I425" s="6"/>
+      <c r="J425" s="3"/>
+      <c r="K425" s="3"/>
+    </row>
+    <row r="426" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B426" s="4"/>
+      <c r="C426" s="2"/>
+      <c r="D426" s="2"/>
+      <c r="E426" s="2"/>
+      <c r="F426" s="5"/>
+      <c r="G426" s="6"/>
+      <c r="H426" s="6"/>
+      <c r="I426" s="6"/>
+      <c r="J426" s="3"/>
+      <c r="K426" s="3"/>
+    </row>
+    <row r="427" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B427" s="4"/>
+      <c r="C427" s="2"/>
+      <c r="D427" s="2"/>
+      <c r="E427" s="2"/>
+      <c r="F427" s="5"/>
+      <c r="G427" s="6"/>
+      <c r="H427" s="6"/>
+      <c r="I427" s="6"/>
+      <c r="J427" s="3"/>
+      <c r="K427" s="3"/>
+    </row>
+    <row r="428" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B428" s="4"/>
+      <c r="C428" s="2"/>
+      <c r="D428" s="2"/>
+      <c r="E428" s="2"/>
+      <c r="F428" s="5"/>
+      <c r="G428" s="6"/>
+      <c r="H428" s="6"/>
+      <c r="I428" s="6"/>
+      <c r="J428" s="3"/>
+      <c r="K428" s="3"/>
+    </row>
+    <row r="429" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B429" s="4"/>
+      <c r="C429" s="2"/>
+      <c r="D429" s="2"/>
+      <c r="E429" s="2"/>
+      <c r="F429" s="5"/>
+      <c r="G429" s="6"/>
+      <c r="H429" s="6"/>
+      <c r="I429" s="6"/>
+      <c r="J429" s="3"/>
+      <c r="K429" s="3"/>
+    </row>
+    <row r="430" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B430" s="4"/>
+      <c r="C430" s="2"/>
+      <c r="D430" s="2"/>
+      <c r="E430" s="2"/>
+      <c r="F430" s="5"/>
+      <c r="G430" s="6"/>
+      <c r="H430" s="6"/>
+      <c r="I430" s="6"/>
+      <c r="J430" s="3"/>
+      <c r="K430" s="3"/>
+    </row>
+    <row r="431" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B431" s="4"/>
+      <c r="C431" s="2"/>
+      <c r="D431" s="2"/>
+      <c r="E431" s="2"/>
+      <c r="F431" s="5"/>
+      <c r="G431" s="6"/>
+      <c r="H431" s="6"/>
+      <c r="I431" s="6"/>
+      <c r="J431" s="3"/>
+      <c r="K431" s="3"/>
+    </row>
+    <row r="432" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B432" s="4"/>
+      <c r="C432" s="2"/>
+      <c r="D432" s="2"/>
+      <c r="E432" s="2"/>
+      <c r="F432" s="5"/>
+      <c r="G432" s="6"/>
+      <c r="H432" s="6"/>
+      <c r="I432" s="6"/>
+      <c r="J432" s="3"/>
+      <c r="K432" s="3"/>
+    </row>
+    <row r="433" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B433" s="4"/>
+      <c r="C433" s="2"/>
+      <c r="D433" s="2"/>
+      <c r="E433" s="2"/>
+      <c r="F433" s="5"/>
+      <c r="G433" s="6"/>
+      <c r="H433" s="6"/>
+      <c r="I433" s="6"/>
+      <c r="J433" s="3"/>
+      <c r="K433" s="3"/>
+    </row>
+    <row r="434" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B434" s="4"/>
+      <c r="C434" s="2"/>
+      <c r="D434" s="2"/>
+      <c r="E434" s="2"/>
+      <c r="F434" s="5"/>
+      <c r="G434" s="6"/>
+      <c r="H434" s="6"/>
+      <c r="I434" s="6"/>
+      <c r="J434" s="3"/>
+      <c r="K434" s="3"/>
+    </row>
+    <row r="435" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B435" s="4"/>
+      <c r="C435" s="2"/>
+      <c r="D435" s="2"/>
+      <c r="E435" s="2"/>
+      <c r="F435" s="5"/>
+      <c r="G435" s="6"/>
+      <c r="H435" s="6"/>
+      <c r="I435" s="6"/>
+      <c r="J435" s="3"/>
+      <c r="K435" s="3"/>
+    </row>
+    <row r="436" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B436" s="4"/>
+      <c r="C436" s="2"/>
+      <c r="D436" s="2"/>
+      <c r="E436" s="2"/>
+      <c r="F436" s="5"/>
+      <c r="G436" s="6"/>
+      <c r="H436" s="6"/>
+      <c r="I436" s="6"/>
+      <c r="J436" s="3"/>
+      <c r="K436" s="3"/>
+    </row>
+    <row r="437" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B437" s="4"/>
+      <c r="C437" s="2"/>
+      <c r="D437" s="2"/>
+      <c r="E437" s="2"/>
+      <c r="F437" s="5"/>
+      <c r="G437" s="6"/>
+      <c r="H437" s="6"/>
+      <c r="I437" s="6"/>
+      <c r="J437" s="3"/>
+      <c r="K437" s="3"/>
+    </row>
+    <row r="438" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B438" s="4"/>
+      <c r="C438" s="2"/>
+      <c r="D438" s="2"/>
+      <c r="E438" s="2"/>
+      <c r="F438" s="5"/>
+      <c r="G438" s="6"/>
+      <c r="H438" s="6"/>
+      <c r="I438" s="6"/>
+      <c r="J438" s="3"/>
+      <c r="K438" s="3"/>
+    </row>
+    <row r="439" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B439" s="4"/>
+      <c r="C439" s="2"/>
+      <c r="D439" s="2"/>
+      <c r="E439" s="2"/>
+      <c r="F439" s="5"/>
+      <c r="G439" s="6"/>
+      <c r="H439" s="6"/>
+      <c r="I439" s="6"/>
+      <c r="J439" s="3"/>
+      <c r="K439" s="3"/>
+    </row>
+    <row r="440" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B440" s="4"/>
+      <c r="C440" s="2"/>
+      <c r="D440" s="2"/>
+      <c r="E440" s="2"/>
+      <c r="F440" s="5"/>
+      <c r="G440" s="6"/>
+      <c r="H440" s="6"/>
+      <c r="I440" s="6"/>
+      <c r="J440" s="3"/>
+      <c r="K440" s="3"/>
+    </row>
+    <row r="441" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B441" s="4"/>
+      <c r="C441" s="2"/>
+      <c r="D441" s="2"/>
+      <c r="E441" s="2"/>
+      <c r="F441" s="5"/>
+      <c r="G441" s="6"/>
+      <c r="H441" s="6"/>
+      <c r="I441" s="6"/>
+      <c r="J441" s="3"/>
+      <c r="K441" s="3"/>
+    </row>
+    <row r="442" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B442" s="4"/>
+      <c r="C442" s="2"/>
+      <c r="D442" s="2"/>
+      <c r="E442" s="2"/>
+      <c r="F442" s="5"/>
+      <c r="G442" s="6"/>
+      <c r="H442" s="6"/>
+      <c r="I442" s="6"/>
+      <c r="J442" s="3"/>
+      <c r="K442" s="3"/>
+    </row>
+    <row r="443" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B443" s="4"/>
+      <c r="C443" s="2"/>
+      <c r="D443" s="2"/>
+      <c r="E443" s="2"/>
+      <c r="F443" s="5"/>
+      <c r="G443" s="6"/>
+      <c r="H443" s="6"/>
+      <c r="I443" s="6"/>
+      <c r="J443" s="3"/>
+      <c r="K443" s="3"/>
+    </row>
+    <row r="444" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B444" s="4"/>
+      <c r="C444" s="2"/>
+      <c r="D444" s="2"/>
+      <c r="E444" s="2"/>
+      <c r="F444" s="5"/>
+      <c r="G444" s="6"/>
+      <c r="H444" s="6"/>
+      <c r="I444" s="6"/>
+      <c r="J444" s="3"/>
+      <c r="K444" s="3"/>
+    </row>
+    <row r="445" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B445" s="4"/>
+      <c r="C445" s="2"/>
+      <c r="D445" s="2"/>
+      <c r="E445" s="2"/>
+      <c r="F445" s="5"/>
+      <c r="G445" s="6"/>
+      <c r="H445" s="6"/>
+      <c r="I445" s="6"/>
+      <c r="J445" s="3"/>
+      <c r="K445" s="3"/>
+    </row>
+    <row r="446" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B446" s="4"/>
+      <c r="C446" s="2"/>
+      <c r="D446" s="2"/>
+      <c r="E446" s="2"/>
+      <c r="F446" s="5"/>
+      <c r="G446" s="6"/>
+      <c r="H446" s="6"/>
+      <c r="I446" s="6"/>
+      <c r="J446" s="3"/>
+      <c r="K446" s="3"/>
+    </row>
+    <row r="447" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B447" s="4"/>
+      <c r="C447" s="2"/>
+      <c r="D447" s="2"/>
+      <c r="E447" s="2"/>
+      <c r="F447" s="5"/>
+      <c r="G447" s="6"/>
+      <c r="H447" s="6"/>
+      <c r="I447" s="6"/>
+      <c r="J447" s="3"/>
+      <c r="K447" s="3"/>
+    </row>
+    <row r="448" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B448" s="4"/>
+      <c r="C448" s="2"/>
+      <c r="D448" s="2"/>
+      <c r="E448" s="2"/>
+      <c r="F448" s="5"/>
+      <c r="G448" s="6"/>
+      <c r="H448" s="6"/>
+      <c r="I448" s="6"/>
+      <c r="J448" s="3"/>
+      <c r="K448" s="3"/>
+    </row>
+    <row r="449" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B449" s="4"/>
+      <c r="C449" s="2"/>
+      <c r="D449" s="2"/>
+      <c r="E449" s="2"/>
+      <c r="F449" s="5"/>
+      <c r="G449" s="6"/>
+      <c r="H449" s="6"/>
+      <c r="I449" s="6"/>
+      <c r="J449" s="3"/>
+      <c r="K449" s="3"/>
+    </row>
+    <row r="450" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B450" s="4"/>
+      <c r="C450" s="2"/>
+      <c r="D450" s="2"/>
+      <c r="E450" s="2"/>
+      <c r="F450" s="5"/>
+      <c r="G450" s="6"/>
+      <c r="H450" s="6"/>
+      <c r="I450" s="6"/>
+      <c r="J450" s="3"/>
+      <c r="K450" s="3"/>
+    </row>
+    <row r="451" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B451" s="4"/>
+      <c r="C451" s="2"/>
+      <c r="D451" s="2"/>
+      <c r="E451" s="2"/>
+      <c r="F451" s="5"/>
+      <c r="G451" s="6"/>
+      <c r="H451" s="6"/>
+      <c r="I451" s="6"/>
+      <c r="J451" s="3"/>
+      <c r="K451" s="3"/>
+    </row>
+    <row r="452" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B452" s="4"/>
+      <c r="C452" s="2"/>
+      <c r="D452" s="2"/>
+      <c r="E452" s="2"/>
+      <c r="F452" s="5"/>
+      <c r="G452" s="6"/>
+      <c r="H452" s="6"/>
+      <c r="I452" s="6"/>
+      <c r="J452" s="3"/>
+      <c r="K452" s="3"/>
+    </row>
+    <row r="453" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B453" s="4"/>
+      <c r="C453" s="2"/>
+      <c r="D453" s="2"/>
+      <c r="E453" s="2"/>
+      <c r="F453" s="5"/>
+      <c r="G453" s="6"/>
+      <c r="H453" s="6"/>
+      <c r="I453" s="6"/>
+      <c r="J453" s="3"/>
+      <c r="K453" s="3"/>
+    </row>
+    <row r="454" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B454" s="4"/>
+      <c r="C454" s="2"/>
+      <c r="D454" s="2"/>
+      <c r="E454" s="2"/>
+      <c r="F454" s="5"/>
+      <c r="G454" s="6"/>
+      <c r="H454" s="6"/>
+      <c r="I454" s="6"/>
+      <c r="J454" s="3"/>
+      <c r="K454" s="3"/>
+    </row>
+    <row r="455" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B455" s="4"/>
+      <c r="C455" s="2"/>
+      <c r="D455" s="2"/>
+      <c r="E455" s="2"/>
+      <c r="F455" s="5"/>
+      <c r="G455" s="6"/>
+      <c r="H455" s="6"/>
+      <c r="I455" s="6"/>
+      <c r="J455" s="3"/>
+      <c r="K455" s="3"/>
+    </row>
+    <row r="456" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B456" s="4"/>
+      <c r="C456" s="2"/>
+      <c r="D456" s="2"/>
+      <c r="E456" s="2"/>
+      <c r="F456" s="5"/>
+      <c r="G456" s="6"/>
+      <c r="H456" s="6"/>
+      <c r="I456" s="6"/>
+      <c r="J456" s="3"/>
+      <c r="K456" s="3"/>
+    </row>
+    <row r="457" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B457" s="4"/>
+      <c r="C457" s="2"/>
+      <c r="D457" s="2"/>
+      <c r="E457" s="2"/>
+      <c r="F457" s="5"/>
+      <c r="G457" s="6"/>
+      <c r="H457" s="6"/>
+      <c r="I457" s="6"/>
+      <c r="J457" s="3"/>
+      <c r="K457" s="3"/>
+    </row>
+    <row r="458" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B458" s="4"/>
+      <c r="C458" s="2"/>
+      <c r="D458" s="2"/>
+      <c r="E458" s="2"/>
+      <c r="F458" s="5"/>
+      <c r="G458" s="6"/>
+      <c r="H458" s="6"/>
+      <c r="I458" s="6"/>
+      <c r="J458" s="3"/>
+      <c r="K458" s="3"/>
+    </row>
+    <row r="459" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B459" s="4"/>
+      <c r="C459" s="2"/>
+      <c r="D459" s="2"/>
+      <c r="E459" s="2"/>
+      <c r="F459" s="5"/>
+      <c r="G459" s="6"/>
+      <c r="H459" s="6"/>
+      <c r="I459" s="6"/>
+      <c r="J459" s="3"/>
+      <c r="K459" s="3"/>
+    </row>
+    <row r="460" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B460" s="4"/>
+      <c r="C460" s="2"/>
+      <c r="D460" s="2"/>
+      <c r="E460" s="2"/>
+      <c r="F460" s="5"/>
+      <c r="G460" s="6"/>
+      <c r="H460" s="6"/>
+      <c r="I460" s="6"/>
+      <c r="J460" s="3"/>
+      <c r="K460" s="3"/>
+    </row>
+    <row r="461" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B461" s="4"/>
+      <c r="C461" s="2"/>
+      <c r="D461" s="2"/>
+      <c r="E461" s="2"/>
+      <c r="F461" s="5"/>
+      <c r="G461" s="6"/>
+      <c r="H461" s="6"/>
+      <c r="I461" s="6"/>
+      <c r="J461" s="3"/>
+      <c r="K461" s="3"/>
+    </row>
+    <row r="462" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B462" s="4"/>
+      <c r="C462" s="2"/>
+      <c r="D462" s="2"/>
+      <c r="E462" s="2"/>
+      <c r="F462" s="5"/>
+      <c r="G462" s="6"/>
+      <c r="H462" s="6"/>
+      <c r="I462" s="6"/>
+      <c r="J462" s="3"/>
+      <c r="K462" s="3"/>
+    </row>
+    <row r="463" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B463" s="4"/>
+      <c r="C463" s="2"/>
+      <c r="D463" s="2"/>
+      <c r="E463" s="2"/>
+      <c r="F463" s="5"/>
+      <c r="G463" s="6"/>
+      <c r="H463" s="6"/>
+      <c r="I463" s="6"/>
+      <c r="J463" s="3"/>
+      <c r="K463" s="3"/>
+    </row>
+    <row r="464" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B464" s="4"/>
+      <c r="C464" s="2"/>
+      <c r="D464" s="2"/>
+      <c r="E464" s="2"/>
+      <c r="F464" s="5"/>
+      <c r="G464" s="6"/>
+      <c r="H464" s="6"/>
+      <c r="I464" s="6"/>
+      <c r="J464" s="3"/>
+      <c r="K464" s="3"/>
+    </row>
+    <row r="465" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B465" s="4"/>
+      <c r="C465" s="2"/>
+      <c r="D465" s="2"/>
+      <c r="E465" s="2"/>
+      <c r="F465" s="5"/>
+      <c r="G465" s="6"/>
+      <c r="H465" s="6"/>
+      <c r="I465" s="6"/>
+      <c r="J465" s="3"/>
+      <c r="K465" s="3"/>
+    </row>
+    <row r="466" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B466" s="4"/>
+      <c r="C466" s="2"/>
+      <c r="D466" s="2"/>
+      <c r="E466" s="2"/>
+      <c r="F466" s="5"/>
+      <c r="G466" s="6"/>
+      <c r="H466" s="6"/>
+      <c r="I466" s="6"/>
+      <c r="J466" s="3"/>
+      <c r="K466" s="3"/>
+    </row>
+    <row r="467" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B467" s="4"/>
+      <c r="C467" s="2"/>
+      <c r="D467" s="2"/>
+      <c r="E467" s="2"/>
+      <c r="F467" s="5"/>
+      <c r="G467" s="6"/>
+      <c r="H467" s="6"/>
+      <c r="I467" s="6"/>
+      <c r="J467" s="3"/>
+      <c r="K467" s="3"/>
+    </row>
+    <row r="468" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B468" s="4"/>
+      <c r="C468" s="2"/>
+      <c r="D468" s="2"/>
+      <c r="E468" s="2"/>
+      <c r="F468" s="5"/>
+      <c r="G468" s="6"/>
+      <c r="H468" s="6"/>
+      <c r="I468" s="6"/>
+      <c r="J468" s="3"/>
+      <c r="K468" s="3"/>
+    </row>
+    <row r="469" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B469" s="4"/>
+      <c r="C469" s="2"/>
+      <c r="D469" s="2"/>
+      <c r="E469" s="2"/>
+      <c r="F469" s="5"/>
+      <c r="G469" s="6"/>
+      <c r="H469" s="6"/>
+      <c r="I469" s="6"/>
+      <c r="J469" s="3"/>
+      <c r="K469" s="3"/>
+    </row>
+    <row r="470" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B470" s="4"/>
+      <c r="C470" s="2"/>
+      <c r="D470" s="2"/>
+      <c r="E470" s="2"/>
+      <c r="F470" s="5"/>
+      <c r="G470" s="6"/>
+      <c r="H470" s="6"/>
+      <c r="I470" s="6"/>
+      <c r="J470" s="3"/>
+      <c r="K470" s="3"/>
+    </row>
+    <row r="471" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B471" s="4"/>
+      <c r="C471" s="2"/>
+      <c r="D471" s="2"/>
+      <c r="E471" s="2"/>
+      <c r="F471" s="5"/>
+      <c r="G471" s="6"/>
+      <c r="H471" s="6"/>
+      <c r="I471" s="6"/>
+      <c r="J471" s="3"/>
+      <c r="K471" s="3"/>
+    </row>
+    <row r="472" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B472" s="4"/>
+      <c r="C472" s="2"/>
+      <c r="D472" s="2"/>
+      <c r="E472" s="2"/>
+      <c r="F472" s="5"/>
+      <c r="G472" s="6"/>
+      <c r="H472" s="6"/>
+      <c r="I472" s="6"/>
+      <c r="J472" s="3"/>
+      <c r="K472" s="3"/>
+    </row>
+    <row r="473" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B473" s="4"/>
+      <c r="C473" s="2"/>
+      <c r="D473" s="2"/>
+      <c r="E473" s="2"/>
+      <c r="F473" s="5"/>
+      <c r="G473" s="6"/>
+      <c r="H473" s="6"/>
+      <c r="I473" s="6"/>
+      <c r="J473" s="3"/>
+      <c r="K473" s="3"/>
+    </row>
+    <row r="474" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B474" s="4"/>
+      <c r="C474" s="2"/>
+      <c r="D474" s="2"/>
+      <c r="E474" s="2"/>
+      <c r="F474" s="5"/>
+      <c r="G474" s="6"/>
+      <c r="H474" s="6"/>
+      <c r="I474" s="6"/>
+      <c r="J474" s="3"/>
+      <c r="K474" s="3"/>
+    </row>
+    <row r="475" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B475" s="4"/>
+      <c r="C475" s="2"/>
+      <c r="D475" s="2"/>
+      <c r="E475" s="2"/>
+      <c r="F475" s="5"/>
+      <c r="G475" s="6"/>
+      <c r="H475" s="6"/>
+      <c r="I475" s="6"/>
+      <c r="J475" s="3"/>
+      <c r="K475" s="3"/>
+    </row>
+    <row r="476" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B476" s="4"/>
+      <c r="C476" s="2"/>
+      <c r="D476" s="2"/>
+      <c r="E476" s="2"/>
+      <c r="F476" s="5"/>
+      <c r="G476" s="6"/>
+      <c r="H476" s="6"/>
+      <c r="I476" s="6"/>
+      <c r="J476" s="3"/>
+      <c r="K476" s="3"/>
+    </row>
+    <row r="477" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B477" s="4"/>
+      <c r="C477" s="2"/>
+      <c r="D477" s="2"/>
+      <c r="E477" s="2"/>
+      <c r="F477" s="5"/>
+      <c r="G477" s="6"/>
+      <c r="H477" s="6"/>
+      <c r="I477" s="6"/>
+      <c r="J477" s="3"/>
+      <c r="K477" s="3"/>
+    </row>
+    <row r="478" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B478" s="4"/>
+      <c r="C478" s="2"/>
+      <c r="D478" s="2"/>
+      <c r="E478" s="2"/>
+      <c r="F478" s="5"/>
+      <c r="G478" s="6"/>
+      <c r="H478" s="6"/>
+      <c r="I478" s="6"/>
+      <c r="J478" s="3"/>
+      <c r="K478" s="3"/>
+    </row>
+    <row r="479" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B479" s="4"/>
+      <c r="C479" s="2"/>
+      <c r="D479" s="2"/>
+      <c r="E479" s="2"/>
+      <c r="F479" s="5"/>
+      <c r="G479" s="6"/>
+      <c r="H479" s="6"/>
+      <c r="I479" s="6"/>
+      <c r="J479" s="3"/>
+      <c r="K479" s="3"/>
+    </row>
+    <row r="480" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B480" s="4"/>
+      <c r="C480" s="2"/>
+      <c r="D480" s="2"/>
+      <c r="E480" s="2"/>
+      <c r="F480" s="5"/>
+      <c r="G480" s="6"/>
+      <c r="H480" s="6"/>
+      <c r="I480" s="6"/>
+      <c r="J480" s="3"/>
+      <c r="K480" s="3"/>
+    </row>
+    <row r="481" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B481" s="4"/>
+      <c r="C481" s="2"/>
+      <c r="D481" s="2"/>
+      <c r="E481" s="2"/>
+      <c r="F481" s="5"/>
+      <c r="G481" s="6"/>
+      <c r="H481" s="6"/>
+      <c r="I481" s="6"/>
+      <c r="J481" s="3"/>
+      <c r="K481" s="3"/>
+    </row>
+    <row r="482" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B482" s="4"/>
+      <c r="C482" s="2"/>
+      <c r="D482" s="2"/>
+      <c r="E482" s="2"/>
+      <c r="F482" s="5"/>
+      <c r="G482" s="6"/>
+      <c r="H482" s="6"/>
+      <c r="I482" s="6"/>
+      <c r="J482" s="3"/>
+      <c r="K482" s="3"/>
+    </row>
+    <row r="483" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B483" s="4"/>
+      <c r="C483" s="2"/>
+      <c r="D483" s="2"/>
+      <c r="E483" s="2"/>
+      <c r="F483" s="5"/>
+      <c r="G483" s="6"/>
+      <c r="H483" s="6"/>
+      <c r="I483" s="6"/>
+      <c r="J483" s="3"/>
+      <c r="K483" s="3"/>
+    </row>
+    <row r="484" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B484" s="4"/>
+      <c r="C484" s="2"/>
+      <c r="D484" s="2"/>
+      <c r="E484" s="2"/>
+      <c r="F484" s="5"/>
+      <c r="G484" s="6"/>
+      <c r="H484" s="6"/>
+      <c r="I484" s="6"/>
+      <c r="J484" s="3"/>
+      <c r="K484" s="3"/>
+    </row>
+    <row r="485" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B485" s="4"/>
+      <c r="C485" s="2"/>
+      <c r="D485" s="2"/>
+      <c r="E485" s="2"/>
+      <c r="F485" s="5"/>
+      <c r="G485" s="6"/>
+      <c r="H485" s="6"/>
+      <c r="I485" s="6"/>
+      <c r="J485" s="3"/>
+      <c r="K485" s="3"/>
+    </row>
+    <row r="486" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B486" s="4"/>
+      <c r="C486" s="2"/>
+      <c r="D486" s="2"/>
+      <c r="E486" s="2"/>
+      <c r="F486" s="5"/>
+      <c r="G486" s="6"/>
+      <c r="H486" s="6"/>
+      <c r="I486" s="6"/>
+      <c r="J486" s="3"/>
+      <c r="K486" s="3"/>
+    </row>
+    <row r="487" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B487" s="4"/>
+      <c r="C487" s="2"/>
+      <c r="D487" s="2"/>
+      <c r="E487" s="2"/>
+      <c r="F487" s="5"/>
+      <c r="G487" s="6"/>
+      <c r="H487" s="6"/>
+      <c r="I487" s="6"/>
+      <c r="J487" s="3"/>
+      <c r="K487" s="3"/>
+    </row>
+    <row r="488" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B488" s="4"/>
+      <c r="C488" s="2"/>
+      <c r="D488" s="2"/>
+      <c r="E488" s="2"/>
+      <c r="F488" s="5"/>
+      <c r="G488" s="6"/>
+      <c r="H488" s="6"/>
+      <c r="I488" s="6"/>
+      <c r="J488" s="3"/>
+      <c r="K488" s="3"/>
+    </row>
+    <row r="489" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B489" s="4"/>
+      <c r="C489" s="2"/>
+      <c r="D489" s="2"/>
+      <c r="E489" s="2"/>
+      <c r="F489" s="5"/>
+      <c r="G489" s="6"/>
+      <c r="H489" s="6"/>
+      <c r="I489" s="6"/>
+      <c r="J489" s="3"/>
+      <c r="K489" s="3"/>
+    </row>
+    <row r="490" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B490" s="4"/>
+      <c r="C490" s="2"/>
+      <c r="D490" s="2"/>
+      <c r="E490" s="2"/>
+      <c r="F490" s="5"/>
+      <c r="G490" s="6"/>
+      <c r="H490" s="6"/>
+      <c r="I490" s="6"/>
+      <c r="J490" s="3"/>
+      <c r="K490" s="3"/>
+    </row>
+    <row r="491" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B491" s="4"/>
+      <c r="C491" s="2"/>
+      <c r="D491" s="2"/>
+      <c r="E491" s="2"/>
+      <c r="F491" s="5"/>
+      <c r="G491" s="6"/>
+      <c r="H491" s="6"/>
+      <c r="I491" s="6"/>
+      <c r="J491" s="3"/>
+      <c r="K491" s="3"/>
+    </row>
+    <row r="492" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B492" s="4"/>
+      <c r="C492" s="2"/>
+      <c r="D492" s="2"/>
+      <c r="E492" s="2"/>
+      <c r="F492" s="5"/>
+      <c r="G492" s="6"/>
+      <c r="H492" s="6"/>
+      <c r="I492" s="6"/>
+      <c r="J492" s="3"/>
+      <c r="K492" s="3"/>
+    </row>
+    <row r="493" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B493" s="4"/>
+      <c r="C493" s="2"/>
+      <c r="D493" s="2"/>
+      <c r="E493" s="2"/>
+      <c r="F493" s="5"/>
+      <c r="G493" s="6"/>
+      <c r="H493" s="6"/>
+      <c r="I493" s="6"/>
+      <c r="J493" s="3"/>
+      <c r="K493" s="3"/>
+    </row>
+    <row r="494" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B494" s="4"/>
+      <c r="C494" s="2"/>
+      <c r="D494" s="2"/>
+      <c r="E494" s="2"/>
+      <c r="F494" s="5"/>
+      <c r="G494" s="6"/>
+      <c r="H494" s="6"/>
+      <c r="I494" s="6"/>
+      <c r="J494" s="3"/>
+      <c r="K494" s="3"/>
+    </row>
+    <row r="495" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B495" s="4"/>
+      <c r="C495" s="2"/>
+      <c r="D495" s="2"/>
+      <c r="E495" s="2"/>
+      <c r="F495" s="5"/>
+      <c r="G495" s="6"/>
+      <c r="H495" s="6"/>
+      <c r="I495" s="6"/>
+      <c r="J495" s="3"/>
+      <c r="K495" s="3"/>
+    </row>
+    <row r="496" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B496" s="4"/>
+      <c r="C496" s="2"/>
+      <c r="D496" s="2"/>
+      <c r="E496" s="2"/>
+      <c r="F496" s="5"/>
+      <c r="G496" s="6"/>
+      <c r="H496" s="6"/>
+      <c r="I496" s="6"/>
+      <c r="J496" s="3"/>
+      <c r="K496" s="3"/>
+    </row>
+    <row r="497" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B497" s="4"/>
+      <c r="C497" s="2"/>
+      <c r="D497" s="2"/>
+      <c r="E497" s="2"/>
+      <c r="F497" s="5"/>
+      <c r="G497" s="6"/>
+      <c r="H497" s="6"/>
+      <c r="I497" s="6"/>
+      <c r="J497" s="3"/>
+      <c r="K497" s="3"/>
+    </row>
+    <row r="498" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B498" s="4"/>
+      <c r="C498" s="2"/>
+      <c r="D498" s="2"/>
+      <c r="E498" s="2"/>
+      <c r="F498" s="5"/>
+      <c r="G498" s="6"/>
+      <c r="H498" s="6"/>
+      <c r="I498" s="6"/>
+      <c r="J498" s="3"/>
+      <c r="K498" s="3"/>
+    </row>
+    <row r="499" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B499" s="4"/>
+      <c r="C499" s="2"/>
+      <c r="D499" s="2"/>
+      <c r="E499" s="2"/>
+      <c r="F499" s="5"/>
+      <c r="G499" s="6"/>
+      <c r="H499" s="6"/>
+      <c r="I499" s="6"/>
+      <c r="J499" s="3"/>
+      <c r="K499" s="3"/>
+    </row>
+    <row r="500" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B500" s="4"/>
+      <c r="C500" s="2"/>
+      <c r="D500" s="2"/>
+      <c r="E500" s="2"/>
+      <c r="F500" s="5"/>
+      <c r="G500" s="6"/>
+      <c r="H500" s="6"/>
+      <c r="I500" s="6"/>
+      <c r="J500" s="3"/>
+      <c r="K500" s="3"/>
+    </row>
+    <row r="501" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B501" s="4"/>
+      <c r="C501" s="2"/>
+      <c r="D501" s="2"/>
+      <c r="E501" s="2"/>
+      <c r="F501" s="5"/>
+      <c r="G501" s="6"/>
+      <c r="H501" s="6"/>
+      <c r="I501" s="6"/>
+      <c r="J501" s="3"/>
+      <c r="K501" s="3"/>
+    </row>
+    <row r="502" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B502" s="4"/>
+      <c r="C502" s="2"/>
+      <c r="D502" s="2"/>
+      <c r="E502" s="2"/>
+      <c r="F502" s="5"/>
+      <c r="G502" s="6"/>
+      <c r="H502" s="6"/>
+      <c r="I502" s="6"/>
+      <c r="J502" s="3"/>
+      <c r="K502" s="3"/>
+    </row>
+    <row r="503" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B503" s="4"/>
+      <c r="C503" s="2"/>
+      <c r="D503" s="2"/>
+      <c r="E503" s="2"/>
+      <c r="F503" s="5"/>
+      <c r="G503" s="6"/>
+      <c r="H503" s="6"/>
+      <c r="I503" s="6"/>
+      <c r="J503" s="3"/>
+      <c r="K503" s="3"/>
+    </row>
+    <row r="504" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B504" s="4"/>
+      <c r="C504" s="2"/>
+      <c r="D504" s="2"/>
+      <c r="E504" s="2"/>
+      <c r="F504" s="5"/>
+      <c r="G504" s="6"/>
+      <c r="H504" s="6"/>
+      <c r="I504" s="6"/>
+      <c r="J504" s="3"/>
+      <c r="K504" s="3"/>
+    </row>
+    <row r="505" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B505" s="4"/>
+      <c r="C505" s="2"/>
+      <c r="D505" s="2"/>
+      <c r="E505" s="2"/>
+      <c r="F505" s="5"/>
+      <c r="G505" s="6"/>
+      <c r="H505" s="6"/>
+      <c r="I505" s="6"/>
+      <c r="J505" s="3"/>
+      <c r="K505" s="3"/>
+    </row>
+    <row r="506" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B506" s="4"/>
+      <c r="C506" s="2"/>
+      <c r="D506" s="2"/>
+      <c r="E506" s="2"/>
+      <c r="F506" s="5"/>
+      <c r="G506" s="6"/>
+      <c r="H506" s="6"/>
+      <c r="I506" s="6"/>
+      <c r="J506" s="3"/>
+      <c r="K506" s="3"/>
+    </row>
+    <row r="507" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B507" s="4"/>
+      <c r="C507" s="2"/>
+      <c r="D507" s="2"/>
+      <c r="E507" s="2"/>
+      <c r="F507" s="5"/>
+      <c r="G507" s="6"/>
+      <c r="H507" s="6"/>
+      <c r="I507" s="6"/>
+      <c r="J507" s="3"/>
+      <c r="K507" s="3"/>
+    </row>
+    <row r="508" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B508" s="4"/>
+      <c r="C508" s="2"/>
+      <c r="D508" s="2"/>
+      <c r="E508" s="2"/>
+      <c r="F508" s="5"/>
+      <c r="G508" s="6"/>
+      <c r="H508" s="6"/>
+      <c r="I508" s="6"/>
+      <c r="J508" s="3"/>
+      <c r="K508" s="3"/>
+    </row>
+    <row r="509" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B509" s="4"/>
+      <c r="C509" s="2"/>
+      <c r="D509" s="2"/>
+      <c r="E509" s="2"/>
+      <c r="F509" s="5"/>
+      <c r="G509" s="6"/>
+      <c r="H509" s="6"/>
+      <c r="I509" s="6"/>
+      <c r="J509" s="3"/>
+      <c r="K509" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>